<commit_message>
[2 18] update ex12a.py
</commit_message>
<xml_diff>
--- a/day2/excel_with_list.xlsx
+++ b/day2/excel_with_list.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="first_sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -363,61 +363,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="D4:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" t="s">
+    <row r="4" spans="4:5">
+      <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="5" spans="4:5">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="E5">
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="6" spans="4:5">
+      <c r="D6" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
+      <c r="E6">
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="7" spans="4:5">
+      <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="E7">
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="8" spans="4:5">
+      <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
+      <c r="E8">
         <v>199</v>
       </c>
     </row>

</xml_diff>